<commit_message>
Added Manual Tests Excel file
</commit_message>
<xml_diff>
--- a/manual-testcases/Assessment_Manual_TestCases.xlsx
+++ b/manual-testcases/Assessment_Manual_TestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -87,11 +87,6 @@
   </si>
   <si>
     <t>Verify that a new user is able to successfully create an account by providing all mandatory information, such as first name, last name, email address, password, and agreeing to the terms and conditions.</t>
-  </si>
-  <si>
-    <t>1.User is on the application’s Registration (Sign-Up) page.
-2.User is not logged into any existing account.
-3.Required fields (like email, password, etc.) are enabled and visible.</t>
   </si>
   <si>
     <t>1. Navigate to the URL https://magento.softwaretestingboard.com/
@@ -119,9 +114,6 @@
     <t>Functional</t>
   </si>
   <si>
-    <t>Yet to Start</t>
-  </si>
-  <si>
     <t>TC_002</t>
   </si>
   <si>
@@ -129,11 +121,6 @@
   </si>
   <si>
     <t>Verify that a registered user is able to log into the application by providing valid credentials.</t>
-  </si>
-  <si>
-    <t>1. User must have a registered account with valid email and password.
-2. User is on the application’s Login page.
-3. User is logged out of any active session.</t>
   </si>
   <si>
     <t>1. Navigate to the URL https://magento.softwaretestingboard.com/
@@ -148,32 +135,6 @@
   </si>
   <si>
     <t>Login</t>
-  </si>
-  <si>
-    <r>
-      <t>Account should be created successfully and user should be redirected to the dashboard with a success message as "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Thank you for registering with Main Website Store.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
   </si>
   <si>
     <r>
@@ -211,11 +172,6 @@
     <t>Verify that a logged-in user can add a product to the shopping cart and proceed to the checkout page successfully.</t>
   </si>
   <si>
-    <t>1. User must be logged in.
-2. Products must be available in the catalog.
-3. Shopping cart must be empty initially.</t>
-  </si>
-  <si>
     <t>1. Navigate to https://magento.softwaretestingboard.com/
 2. Log in with valid credentials.
 3. Select any product from the home page .
@@ -242,11 +198,6 @@
   </si>
   <si>
     <t>Verify that a registered user can add a product to the cart, place an order successfully, and verify the order details from 'My Orders' section.</t>
-  </si>
-  <si>
-    <t>1. User must be registered and logged in.
-2. At least one product must be available in cart.
-3. User should have valid shipping address and valid shipping method selected</t>
   </si>
   <si>
     <t>1. Navigate to https://magento.softwaretestingboard.com/
@@ -288,23 +239,111 @@
     <t>User must have an existing account with a valid email address</t>
   </si>
   <si>
-    <t>1. Go to the login page
+    <t>Registered Email: johndoe@test.com
+New Password: NewTest@1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Account Recovery</t>
+  </si>
+  <si>
+    <r>
+      <t>Account should be created successfully and user should be redirected to the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> My Accounts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page with a success message as "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thank you for registering with Main Website Store.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Navigate to https://magento.softwaretestingboard.com/customer/account/login
 2. Click "Forgot Your Password?" link
 3. Enter registered email address
-4. Submit reset request
+4. click on Reset my Password button
 5. Open email and click the password reset link
 6. Enter new password and confirm
 7. Submit the new password</t>
   </si>
   <si>
-    <t>Registered Email: johndoe@test.com
-New Password: NewTest@1234</t>
-  </si>
-  <si>
-    <t>User receives a password reset email, successfully resets the password, and can log in with the new password.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Account Recovery</t>
+    <r>
+      <t>1.Once user clicks on the Rest my Password button user should be redirected to the Sign Page and the message should be displayed as "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If there is an account associated with anandjeyakumar7@gmail.com you will receive an email with a link to reset your password.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"                 2.User receives a password reset email, successfully resets the password, and can log in with the new password.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1..User is not logged into any existing account.
+2.Required fields (like email, password, etc.) are enabled and visible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Products must be available in the catalog.
+2. Shopping cart must be empty initially.</t>
+  </si>
+  <si>
+    <t>1. User must have a registered account with valid email and password.
+2. User is logged out of any active session.</t>
+  </si>
+  <si>
+    <t>1. User must be registered .
+2. At least one product must be available in cart.</t>
   </si>
 </sst>
 </file>
@@ -336,7 +375,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -344,15 +383,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -360,8 +439,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,377 +730,379 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="49" style="2" customWidth="1"/>
-    <col min="4" max="4" width="37.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="52.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.26953125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.08984375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="10.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.08984375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="174" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="K2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" t="s">
+      <c r="D4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="L4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="1:18" ht="145" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" ht="232" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="L5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" ht="232" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="L6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="M6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="A7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>